<commit_message>
added create account tests
</commit_message>
<xml_diff>
--- a/test_data/Data_magento.xlsx
+++ b/test_data/Data_magento.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\EI_Python_Training\CaptionProject\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E9B87C-B10B-4F49-9B87-715510138483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6289F931-3C40-470A-B960-EE54B55394B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invalid_login_test" sheetId="1" r:id="rId1"/>
     <sheet name="Products" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId3"/>
+    <sheet name="create_account" sheetId="4" r:id="rId3"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId5"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>username</t>
   </si>
@@ -65,13 +65,55 @@
   </si>
   <si>
     <t>Fitness Equipment</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>confirmpassword</t>
+  </si>
+  <si>
+    <t>jack</t>
+  </si>
+  <si>
+    <t>sparrow</t>
+  </si>
+  <si>
+    <t>jack@email.com</t>
+  </si>
+  <si>
+    <t>1qweae</t>
+  </si>
+  <si>
+    <t>errormessage</t>
+  </si>
+  <si>
+    <t>Minimum length of this field must be equal or greater than 8 symbols. Leading and trailing spaces will be ignored.</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>wick</t>
+  </si>
+  <si>
+    <t>wick@email.com</t>
+  </si>
+  <si>
+    <t>Minimum of different classes of characters in password is 3. Classes of characters: Lower Case, Upper Case, Digits, Special Characters.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -86,6 +128,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,9 +157,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -458,7 +507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -494,13 +543,84 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="22.6328125" customWidth="1"/>
+    <col min="4" max="4" width="24.08984375" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" customWidth="1"/>
+    <col min="6" max="6" width="49.7265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="52.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3">
+        <v>112233445566</v>
+      </c>
+      <c r="F3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="D4" s="2"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{391C9407-80C3-4895-ADBC-80FDB60B22C0}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{E8E24FD5-5234-449C-AE9F-F257A6DF21A9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>